<commit_message>
more data and post-procesing
</commit_message>
<xml_diff>
--- a/Data/A147_scope_2021_05_17.xlsx
+++ b/Data/A147_scope_2021_05_17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMW63\Desktop\R_Projects\scope_qpcr_analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3FA031-0B5C-46DF-9C42-5036E551B52B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15064EF6-57DD-4C4D-A60B-F1073A297F9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="2840" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A147_scope_2021_05_17" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>A09</t>
   </si>
   <si>
-    <t>46.9</t>
-  </si>
-  <si>
     <t>A10</t>
   </si>
   <si>
@@ -437,6 +434,9 @@
   </si>
   <si>
     <t>-5</t>
+  </si>
+  <si>
+    <t>46.2</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -545,6 +545,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -863,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1201,8 +1204,8 @@
       <c r="D29" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>54</v>
+      <c r="E29" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>38</v>
@@ -1210,19 +1213,19 @@
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>38</v>
@@ -1230,19 +1233,19 @@
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>38</v>
@@ -1250,19 +1253,19 @@
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>38</v>
@@ -1270,19 +1273,19 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>38</v>
@@ -1290,19 +1293,19 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>38</v>
@@ -1310,19 +1313,19 @@
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>38</v>
@@ -1330,19 +1333,19 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>38</v>
@@ -1350,19 +1353,19 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>38</v>
@@ -1370,19 +1373,19 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>38</v>
@@ -1390,19 +1393,19 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>38</v>
@@ -1410,19 +1413,19 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>38</v>
@@ -1430,19 +1433,19 @@
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>38</v>
@@ -1450,19 +1453,19 @@
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>38</v>
@@ -1470,19 +1473,19 @@
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>38</v>
@@ -1490,19 +1493,19 @@
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>38</v>
@@ -1510,19 +1513,19 @@
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>38</v>
@@ -1530,19 +1533,19 @@
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>38</v>
@@ -1550,19 +1553,19 @@
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>38</v>
@@ -1570,19 +1573,19 @@
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>38</v>
@@ -1590,19 +1593,19 @@
     </row>
     <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>38</v>
@@ -1610,19 +1613,19 @@
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>38</v>
@@ -1630,19 +1633,19 @@
     </row>
     <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>38</v>
@@ -1650,19 +1653,19 @@
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>38</v>
@@ -1670,19 +1673,19 @@
     </row>
     <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>38</v>
@@ -1690,19 +1693,19 @@
     </row>
     <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>38</v>
@@ -1710,19 +1713,19 @@
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>38</v>
@@ -1733,19 +1736,19 @@
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>38</v>
@@ -1753,19 +1756,19 @@
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>38</v>
@@ -1773,19 +1776,19 @@
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>38</v>
@@ -1793,19 +1796,19 @@
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>38</v>
@@ -1813,19 +1816,19 @@
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>38</v>
@@ -1833,19 +1836,19 @@
     </row>
     <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>38</v>
@@ -1853,19 +1856,19 @@
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>38</v>
@@ -1873,7 +1876,7 @@
     </row>
     <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>34</v>
@@ -1884,7 +1887,7 @@
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>34</v>
@@ -1895,7 +1898,7 @@
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>34</v>
@@ -1906,7 +1909,7 @@
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>34</v>
@@ -1917,7 +1920,7 @@
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>34</v>
@@ -1928,16 +1931,16 @@
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>35</v>
@@ -1948,19 +1951,19 @@
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D69" s="7" t="s">
+      <c r="E69" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>38</v>
@@ -1971,19 +1974,19 @@
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E70" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>38</v>
@@ -1994,19 +1997,19 @@
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E71" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>38</v>
@@ -2017,19 +2020,19 @@
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E72" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>38</v>
@@ -2040,19 +2043,19 @@
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E73" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>38</v>

</xml_diff>